<commit_message>
Security Commit before changing Combobox Template
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{588F9B31-1D1D-4BFE-8E1C-BD6EEE50CE38}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9574F946-2DF2-4126-87D0-95A5E7B7277E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>14.11.17</t>
   </si>
@@ -105,6 +105,20 @@
   <si>
     <t>-App-Resources (GUI Design)
 -Preperations of Input Options</t>
+  </si>
+  <si>
+    <t>20.10.18</t>
+  </si>
+  <si>
+    <t>-App-Resources (GUI Design)
+-WMI for list of available cameras</t>
+  </si>
+  <si>
+    <t>21.10.18</t>
+  </si>
+  <si>
+    <t>massive timesink on custom styles and templates
+reading up + tutorials</t>
   </si>
 </sst>
 </file>
@@ -139,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -199,11 +213,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -230,6 +270,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,7 +560,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,6 +569,7 @@
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -753,38 +800,56 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="C13" s="4">
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="0"/>
-        <v>0.27083333333333331</v>
+        <v>0.22916666666666669</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.75</v>
+      </c>
       <c r="D14" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+        <v>0.20833333333333337</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.75</v>
+      </c>
       <c r="D15" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="1"/>
+        <v>0.1875</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -904,13 +969,14 @@
       <c r="C26" s="14"/>
       <c r="D26" s="8">
         <f>SUM(D3:D25)</f>
-        <v>1.7604166666666667</v>
+        <v>2.1145833333333335</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added WMI query to get list of available cameras
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9574F946-2DF2-4126-87D0-95A5E7B7277E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8D8C473B-0F2B-4FC0-B542-B7620AD7ABF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>14.11.17</t>
   </si>
@@ -119,6 +119,15 @@
   <si>
     <t>massive timesink on custom styles and templates
 reading up + tutorials</t>
+  </si>
+  <si>
+    <t>25. 10.18</t>
+  </si>
+  <si>
+    <t>-Issues with WMI</t>
+  </si>
+  <si>
+    <t>26. 10.18</t>
   </si>
 </sst>
 </file>
@@ -271,11 +280,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +569,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,7 +837,7 @@
       <c r="E14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>30</v>
       </c>
     </row>
@@ -849,28 +858,44 @@
       <c r="E15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="D16" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="D17" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -969,7 +994,7 @@
       <c r="C26" s="14"/>
       <c r="D26" s="8">
         <f>SUM(D3:D25)</f>
-        <v>2.1145833333333335</v>
+        <v>2.2395833333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-made general options and cameraviewmodel singleton -added load buttoons for xml cascade files for face and eyedetection, so they don't need to be hardcoded in the future (still have to implement this feature into the cascade detector)
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8D8C473B-0F2B-4FC0-B542-B7620AD7ABF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A03ED553-B254-4417-AEA9-89235EF3644A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>14.11.17</t>
   </si>
@@ -128,6 +128,10 @@
   </si>
   <si>
     <t>26. 10.18</t>
+  </si>
+  <si>
+    <t>-Cascasde-Classifier Options and refactoring
+-Timer</t>
   </si>
 </sst>
 </file>
@@ -569,7 +573,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,15 +902,23 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="D18" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="6"/>
+        <v>0.125</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -994,7 +1006,7 @@
       <c r="C26" s="14"/>
       <c r="D26" s="8">
         <f>SUM(D3:D25)</f>
-        <v>2.2395833333333335</v>
+        <v>2.3645833333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit for safety: -improved loading of xml-files -prepared color picker for eye and face rectangles
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A03ED553-B254-4417-AEA9-89235EF3644A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1997D1F-3550-4A44-A6E1-B5E0E1D0ED60}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>14.11.17</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>26. 10.18</t>
+  </si>
+  <si>
+    <t>-Cascasde-Classifier Options and refactoring</t>
+  </si>
+  <si>
+    <t>30.10.18</t>
+  </si>
+  <si>
+    <t>31.10.18</t>
   </si>
   <si>
     <t>-Cascasde-Classifier Options and refactoring
@@ -573,7 +582,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,34 +911,42 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B18" s="4">
         <v>0.66666666666666663</v>
       </c>
       <c r="C18" s="4">
-        <v>0.79166666666666663</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.375E-2</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.75</v>
+      </c>
       <c r="D19" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="6"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1006,7 +1023,7 @@
       <c r="C26" s="14"/>
       <c r="D26" s="8">
         <f>SUM(D3:D25)</f>
-        <v>2.3645833333333335</v>
+        <v>2.625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added calculation for Angle between the eyes
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2795D13-1F00-499E-95AF-6C66B62A6A91}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7E58B6DE-314B-4B26-825F-E608E4574CB1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>14.11.17</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>31.10.18</t>
+  </si>
+  <si>
+    <t>01.11.18</t>
+  </si>
+  <si>
+    <t>-Add Point angle calculation</t>
   </si>
 </sst>
 </file>
@@ -578,7 +584,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,14 +952,22 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="D20" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1019,7 +1033,7 @@
       <c r="C26" s="14"/>
       <c r="D26" s="8">
         <f>SUM(D3:D25)</f>
-        <v>2.625</v>
+        <v>2.6875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleanup of Detect method arguments
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7E58B6DE-314B-4B26-825F-E608E4574CB1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4D80AA22-794E-4DAE-926B-EDB0AB74D55A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>14.11.17</t>
   </si>
@@ -142,7 +142,13 @@
     <t>01.11.18</t>
   </si>
   <si>
-    <t>-Add Point angle calculation</t>
+    <t>-Add eyes angle calculation</t>
+  </si>
+  <si>
+    <t>11.11.18</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -584,7 +590,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,11 +965,11 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C20" s="4">
-        <v>0.77083333333333337</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="D20" s="9">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>9.375E-2</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>38</v>
@@ -971,14 +977,22 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.6875</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.875</v>
+      </c>
       <c r="D21" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="6"/>
+        <v>0.1875</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1033,7 +1047,7 @@
       <c r="C26" s="14"/>
       <c r="D26" s="8">
         <f>SUM(D3:D25)</f>
-        <v>2.6875</v>
+        <v>2.90625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Preparation of OutpuOptions -NextStep Implementation of OutputOptions
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4D80AA22-794E-4DAE-926B-EDB0AB74D55A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{80039849-584D-4046-A8EE-9E76F50F5E40}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,9 @@
     <t>11.11.18</t>
   </si>
   <si>
-    <t>-</t>
+    <t>-Added timer
+-Added Options for Idling after frame calculation
+-Prepared OutputOptions</t>
   </si>
 </sst>
 </file>
@@ -976,7 +978,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
@@ -984,13 +986,13 @@
         <v>0.6875</v>
       </c>
       <c r="C21" s="4">
-        <v>0.875</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D21" s="9">
         <f t="shared" si="0"/>
-        <v>0.1875</v>
-      </c>
-      <c r="E21" s="6" t="s">
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="1"/>
@@ -1047,7 +1049,7 @@
       <c r="C26" s="14"/>
       <c r="D26" s="8">
         <f>SUM(D3:D25)</f>
-        <v>2.90625</v>
+        <v>2.8645833333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Prepared and Implemented Content Control for different OuptutOptionsViews
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{80039849-584D-4046-A8EE-9E76F50F5E40}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{95D16408-712D-412A-B3BC-8E0AF1E71221}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>14.11.17</t>
   </si>
@@ -151,6 +151,12 @@
     <t>-Added timer
 -Added Options for Idling after frame calculation
 -Prepared OutputOptions</t>
+  </si>
+  <si>
+    <t>12.11.18</t>
+  </si>
+  <si>
+    <t>-Output Options</t>
   </si>
 </sst>
 </file>
@@ -592,7 +598,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,14 +1004,22 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.75</v>
+      </c>
       <c r="D22" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="6"/>
+        <v>0.3125</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1049,7 +1063,7 @@
       <c r="C26" s="14"/>
       <c r="D26" s="8">
         <f>SUM(D3:D25)</f>
-        <v>2.8645833333333335</v>
+        <v>3.1770833333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit for safety before Interfaces
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{95D16408-712D-412A-B3BC-8E0AF1E71221}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{18D291CC-40A8-4331-A678-09BD38243701}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>14.11.17</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>-Output Options</t>
+  </si>
+  <si>
+    <t>13.11.18</t>
+  </si>
+  <si>
+    <t>-Mouse Button Simulation</t>
   </si>
 </sst>
 </file>
@@ -598,7 +604,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,11 +1017,11 @@
         <v>0.4375</v>
       </c>
       <c r="C22" s="4">
-        <v>0.75</v>
+        <v>0.78125</v>
       </c>
       <c r="D22" s="9">
         <f t="shared" si="0"/>
-        <v>0.3125</v>
+        <v>0.34375</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>42</v>
@@ -1023,14 +1029,22 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="D23" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="6"/>
+        <v>0.125</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1063,7 +1077,7 @@
       <c r="C26" s="14"/>
       <c r="D26" s="8">
         <f>SUM(D3:D25)</f>
-        <v>3.1770833333333335</v>
+        <v>3.3333333333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Problem with databinding solved
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{18D291CC-40A8-4331-A678-09BD38243701}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{08D694FF-4E68-4CD7-BD38-BD2017951973}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>14.11.17</t>
   </si>
@@ -162,7 +162,13 @@
     <t>13.11.18</t>
   </si>
   <si>
-    <t>-Mouse Button Simulation</t>
+    <t>14.11.18</t>
+  </si>
+  <si>
+    <t>-Implementation of TriggerEvent</t>
+  </si>
+  <si>
+    <t>-Preparing OutputOptions</t>
   </si>
 </sst>
 </file>
@@ -601,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +682,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D25" si="0">C4-B4</f>
+        <f t="shared" ref="D4:D30" si="0">C4-B4</f>
         <v>0.10416666666666663</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1024,7 +1030,7 @@
         <v>0.34375</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1043,47 +1049,95 @@
         <v>0.125</v>
       </c>
       <c r="E23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="B24" s="4">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.84375</v>
+      </c>
       <c r="D24" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="6"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D25" s="9"/>
       <c r="E25" s="6"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="8">
-        <f>SUM(D3:D25)</f>
-        <v>3.3333333333333335</v>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="8">
+        <f>SUM(D3:D30)</f>
+        <v>3.75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A31:C31"/>
     <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
-refactoring -using webeye framework to detect available cameras
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{057AAD1A-BCB0-46AA-B80C-FE816E457D5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ED910EDE-4EBF-4CE8-93CC-FC8DB9FA43F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>14.11.17</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>-refactoring</t>
+  </si>
+  <si>
+    <t>19.11.18</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,11 +1114,11 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="C26" s="4">
-        <v>0.63541666666666663</v>
+        <v>0.59375</v>
       </c>
       <c r="D26" s="9">
         <f t="shared" si="0"/>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>50</v>
@@ -1123,11 +1126,22 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="6"/>
+      <c r="A27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" si="0"/>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1205,7 +1219,7 @@
       <c r="C36" s="14"/>
       <c r="D36" s="8">
         <f>SUM(D3:D35)</f>
-        <v>4.208333333333333</v>
+        <v>4.4583333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Squirrel updater (testing now, full functionality will follow)
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{109C325E-7663-4DAD-BC57-42445134C99F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5270F6EA-1BD6-4ACA-8F14-22B75EDC4C36}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,11 +1183,11 @@
         <v>0.5</v>
       </c>
       <c r="C29" s="4">
-        <v>0.75</v>
+        <v>0.6875</v>
       </c>
       <c r="D29" s="9">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.1875</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>55</v>
@@ -1250,7 +1250,7 @@
       <c r="C36" s="14"/>
       <c r="D36" s="8">
         <f>SUM(D3:D35)</f>
-        <v>4.7500000000000009</v>
+        <v>4.6875000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-started with keypresssequence simultation
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5270F6EA-1BD6-4ACA-8F14-22B75EDC4C36}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{706640AE-68DC-43B1-ACAA-2560D62C1957}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>14.11.17</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>-reading up on app deployment (squirrel)</t>
+  </si>
+  <si>
+    <t>24.11.18</t>
+  </si>
+  <si>
+    <t>-squirrel</t>
+  </si>
+  <si>
+    <t>26.11.18</t>
   </si>
 </sst>
 </file>
@@ -637,7 +646,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +718,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D29" si="0">C4-B4</f>
+        <f t="shared" ref="D4:D31" si="0">C4-B4</f>
         <v>0.10416666666666663</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1195,19 +1204,41 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="6"/>
+      <c r="A30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D30" s="9">
+        <f t="shared" si="0"/>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D31" s="9">
+        <f t="shared" si="0"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1250,7 +1281,7 @@
       <c r="C36" s="14"/>
       <c r="D36" s="8">
         <f>SUM(D3:D35)</f>
-        <v>4.6875000000000009</v>
+        <v>5.2291666666666679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Keypress sequence done except for the trigger activation and actual simulation
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{706640AE-68DC-43B1-ACAA-2560D62C1957}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3C26DD74-07F5-46FC-92F3-E86C3467F09C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>14.11.17</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>26.11.18</t>
+  </si>
+  <si>
+    <t>28.11.18</t>
   </si>
 </sst>
 </file>
@@ -643,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +721,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D31" si="0">C4-B4</f>
+        <f t="shared" ref="D4:D32" si="0">C4-B4</f>
         <v>0.10416666666666663</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1242,11 +1245,22 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="6"/>
+      <c r="A32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.65625</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D32" s="9">
+        <f t="shared" si="0"/>
+        <v>0.13541666666666663</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1274,20 +1288,52 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="8">
-        <f>SUM(D3:D35)</f>
-        <v>5.2291666666666679</v>
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="8">
+        <f>SUM(D3:D39)</f>
+        <v>5.3645833333333348</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commit for safety before creating datagrid template
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3C26DD74-07F5-46FC-92F3-E86C3467F09C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1AE6730E-F5CB-43AD-BE4C-02EF7E7F463B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>14.11.17</t>
   </si>
@@ -208,6 +208,13 @@
   </si>
   <si>
     <t>28.11.18</t>
+  </si>
+  <si>
+    <t>01.12.18</t>
+  </si>
+  <si>
+    <t>-Open External Software
+-Tooltipps</t>
   </si>
 </sst>
 </file>
@@ -649,7 +656,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +728,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D32" si="0">C4-B4</f>
+        <f t="shared" ref="D4:D33" si="0">C4-B4</f>
         <v>0.10416666666666663</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1263,12 +1270,23 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="6"/>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D33" s="9">
+        <f t="shared" si="0"/>
+        <v>0.31249999999999994</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1327,7 +1345,7 @@
       <c r="C40" s="14"/>
       <c r="D40" s="8">
         <f>SUM(D3:D39)</f>
-        <v>5.3645833333333348</v>
+        <v>5.6770833333333348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Open External Softwar working
</commit_message>
<xml_diff>
--- a/VisualDetection/!diary.xlsx
+++ b/VisualDetection/!diary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1AE6730E-F5CB-43AD-BE4C-02EF7E7F463B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{80C4274B-CB8F-4E76-8637-ABF7CF039A70}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>14.11.17</t>
   </si>
@@ -215,6 +215,9 @@
   <si>
     <t>-Open External Software
 -Tooltipps</t>
+  </si>
+  <si>
+    <t>02.12.18</t>
   </si>
 </sst>
 </file>
@@ -656,7 +659,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +731,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D33" si="0">C4-B4</f>
+        <f t="shared" ref="D4:D34" si="0">C4-B4</f>
         <v>0.10416666666666663</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1289,12 +1292,23 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="6"/>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D34" s="9">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1345,7 +1359,7 @@
       <c r="C40" s="14"/>
       <c r="D40" s="8">
         <f>SUM(D3:D39)</f>
-        <v>5.6770833333333348</v>
+        <v>6.0104166666666679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>